<commit_message>
update excel output script with xlsm
</commit_message>
<xml_diff>
--- a/src/analysis/output_templates/output_template.xlsx
+++ b/src/analysis/output_templates/output_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2231c577fa22c521/WS2022/ENS_Panda/PROENS/src/analysis/output_templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Documents\propens-pandapower\src\analysis\output_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{8EDB1137-6AA4-451B-8281-3790142075D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{1430554A-E4D2-4B84-BBE8-57A1A47EEA38}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DF9C76-D69D-450F-90AC-2297BF67D3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11235" activeTab="6" xr2:uid="{DD082620-07CE-4DCC-8FD9-64D878DA0543}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{DD082620-07CE-4DCC-8FD9-64D878DA0543}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
@@ -29,9 +29,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Buses!$C$3:$J$3</definedName>
     <definedName name="Slicer_Fuel">#N/A</definedName>
     <definedName name="Slicer_Technology">#N/A</definedName>
-    <definedName name="Slicer_Voltage_Level__kV">#N/A</definedName>
     <definedName name="Slicer_Voltage_Level__kV1">#N/A</definedName>
-    <definedName name="Slicer_Zone">#N/A</definedName>
     <definedName name="Slicer_Zone1">#N/A</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -46,8 +44,6 @@
         <x14:slicerCache r:id="rId15"/>
         <x14:slicerCache r:id="rId16"/>
         <x14:slicerCache r:id="rId17"/>
-        <x14:slicerCache r:id="rId18"/>
-        <x14:slicerCache r:id="rId19"/>
       </x14:slicerCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -59,9 +55,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -70,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="78">
   <si>
     <t>Zone</t>
   </si>
@@ -160,9 +154,6 @@
   </si>
   <si>
     <t>Std. Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            </t>
   </si>
   <si>
     <t>From Bus Act. Power [MW]</t>
@@ -306,34 +297,7 @@
     <t>Sum of Losses [MW]</t>
   </si>
   <si>
-    <t>Summary</t>
-  </si>
-  <si>
-    <t>Line Overloaded</t>
-  </si>
-  <si>
-    <t>Line</t>
-  </si>
-  <si>
-    <t>Used Percentage</t>
-  </si>
-  <si>
-    <t>Voltage Violation in Bus</t>
-  </si>
-  <si>
-    <t>Bus</t>
-  </si>
-  <si>
-    <t>Voltage</t>
-  </si>
-  <si>
-    <t>Over/Under</t>
-  </si>
-  <si>
-    <t>Trafo Overloaded</t>
-  </si>
-  <si>
-    <t>Trafo</t>
+    <t>0.25 MVA 10/0.4 kV</t>
   </si>
 </sst>
 </file>
@@ -433,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -465,10 +429,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,7 +466,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="ko-KR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2593,7 +2554,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="ko-KR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3747,7 +3708,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="ko-KR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6005,7 +5966,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="ko-KR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -9337,84 +9298,6 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>34738</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>34738</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:graphicFrame macro="">
-          <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="3" name="Zone">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51BCC28D-B75C-61DA-C582-86F4A8A7F6C3}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvGraphicFramePr/>
-          </xdr:nvGraphicFramePr>
-          <xdr:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="0" cy="0"/>
-          </xdr:xfrm>
-          <a:graphic>
-            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
-              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Zone"/>
-            </a:graphicData>
-          </a:graphic>
-        </xdr:graphicFrame>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
-            <xdr:cNvSpPr>
-              <a:spLocks noTextEdit="1"/>
-            </xdr:cNvSpPr>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="941518" y="1082040"/>
-              <a:ext cx="1828800" cy="2539365"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:prstClr val="white"/>
-            </a:solidFill>
-            <a:ln w="1">
-              <a:solidFill>
-                <a:prstClr val="green"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
-                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
-If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
       <xdr:colOff>23532</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>144556</xdr:rowOff>
@@ -9539,84 +9422,6 @@
             <a:xfrm>
               <a:off x="2805280" y="3655919"/>
               <a:ext cx="1830705" cy="2522220"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:prstClr val="white"/>
-            </a:solidFill>
-            <a:ln w="1">
-              <a:solidFill>
-                <a:prstClr val="green"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
-                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
-If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>72838</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>58831</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>72838</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>110266</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:graphicFrame macro="">
-          <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="6" name="Voltage Level [kV]">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{436C9F94-124E-10A1-6DAB-3D4F5B956097}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvGraphicFramePr/>
-          </xdr:nvGraphicFramePr>
-          <xdr:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="0" cy="0"/>
-          </xdr:xfrm>
-          <a:graphic>
-            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
-              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Voltage Level [kV]"/>
-            </a:graphicData>
-          </a:graphic>
-        </xdr:graphicFrame>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
-            <xdr:cNvSpPr>
-              <a:spLocks noTextEdit="1"/>
-            </xdr:cNvSpPr>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2808418" y="1098961"/>
-              <a:ext cx="1828800" cy="2524125"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -13395,22 +13200,6 @@
 </file>
 
 <file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Zone" xr10:uid="{81A1CE24-8171-4E96-9C9E-C69C801D78B5}" sourceName="Zone">
-  <pivotTables>
-    <pivotTable tabId="9" name="PivotTable16"/>
-    <pivotTable tabId="10" name="PivotTable1"/>
-  </pivotTables>
-  <data>
-    <tabular pivotCacheId="1923745019">
-      <items count="1">
-        <i x="0" s="1"/>
-      </items>
-    </tabular>
-  </data>
-</slicerCacheDefinition>
-</file>
-
-<file path=xl/slicerCaches/slicerCache2.xml><?xml version="1.0" encoding="utf-8"?>
 <slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Fuel" xr10:uid="{E08D1685-E2A5-4C03-B51C-A36B18FEA8F0}" sourceName="Fuel">
   <pivotTables>
     <pivotTable tabId="9" name="PivotTable16"/>
@@ -13428,7 +13217,7 @@
 </slicerCacheDefinition>
 </file>
 
-<file path=xl/slicerCaches/slicerCache3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/slicerCaches/slicerCache2.xml><?xml version="1.0" encoding="utf-8"?>
 <slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Technology" xr10:uid="{DCA87D60-13B1-43E0-A15D-B5424B376629}" sourceName="Technology">
   <pivotTables>
     <pivotTable tabId="9" name="PivotTable16"/>
@@ -13446,24 +13235,7 @@
 </slicerCacheDefinition>
 </file>
 
-<file path=xl/slicerCaches/slicerCache4.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Voltage_Level__kV" xr10:uid="{CF358931-9FFB-4F4B-9AF0-97E07AA439D3}" sourceName="Voltage Level [kV]">
-  <pivotTables>
-    <pivotTable tabId="9" name="PivotTable16"/>
-    <pivotTable tabId="10" name="PivotTable1"/>
-  </pivotTables>
-  <data>
-    <tabular pivotCacheId="1923745019">
-      <items count="2">
-        <i x="1" s="1"/>
-        <i x="0" s="1"/>
-      </items>
-    </tabular>
-  </data>
-</slicerCacheDefinition>
-</file>
-
-<file path=xl/slicerCaches/slicerCache5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/slicerCaches/slicerCache3.xml><?xml version="1.0" encoding="utf-8"?>
 <slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Zone1" xr10:uid="{68A43A06-6138-4CB3-86D8-B1FC89E2D1A7}" sourceName="Zone">
   <pivotTables>
     <pivotTable tabId="11" name="PivotTable2"/>
@@ -13479,7 +13251,7 @@
 </slicerCacheDefinition>
 </file>
 
-<file path=xl/slicerCaches/slicerCache6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/slicerCaches/slicerCache4.xml><?xml version="1.0" encoding="utf-8"?>
 <slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Voltage_Level__kV1" xr10:uid="{F2BE660A-006C-425A-9F04-9E5F550333B3}" sourceName="Voltage Level [kV]">
   <pivotTables>
     <pivotTable tabId="11" name="PivotTable2"/>
@@ -13498,10 +13270,8 @@
 
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
-  <slicer name="Zone" xr10:uid="{BDABF252-F4E4-449D-919F-CE436EAA7841}" cache="Slicer_Zone" caption="Zone" rowHeight="241300"/>
   <slicer name="Fuel" xr10:uid="{D74C6C14-73FC-4D6E-B99C-6FB6E77FFCFD}" cache="Slicer_Fuel" caption="Fuel" rowHeight="241300"/>
   <slicer name="Technology" xr10:uid="{10460025-1A94-432B-8351-071CE786F7CE}" cache="Slicer_Technology" caption="Technology" rowHeight="241300"/>
-  <slicer name="Voltage Level [kV]" xr10:uid="{9639BAED-61AC-4802-A727-B4C39FF4B5FD}" cache="Slicer_Voltage_Level__kV" caption="Voltage Level [kV]" rowHeight="241300"/>
   <slicer name="Zone 1" xr10:uid="{F51052F0-AFB3-4B80-9842-C0E7094EE4BC}" cache="Slicer_Zone1" caption="Zone" rowHeight="241300"/>
   <slicer name="Voltage Level [kV] 1" xr10:uid="{0917183F-F97E-4FB5-AD51-DBD383B70248}" cache="Slicer_Voltage_Level__kV1" caption="Voltage Level [kV]" rowHeight="241300"/>
 </slicers>
@@ -13924,75 +13694,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A97B7531-FB9D-4A11-8F8E-0B25BAB0D225}">
-  <dimension ref="B2:L11"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>87</v>
-      </c>
-      <c r="C11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:D2"/>
-  </mergeCells>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -14001,24 +13710,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{498B9BF1-1E58-4308-B5FF-BD4802D2FFBD}">
   <dimension ref="B2:U69"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W55" sqref="W55"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="11" max="11" width="10.7109375" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" customWidth="1"/>
+    <col min="16" max="16" width="12.88671875" customWidth="1"/>
     <col min="17" max="17" width="12" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" customWidth="1"/>
+    <col min="18" max="18" width="12.88671875" customWidth="1"/>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:21" ht="21" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
         <v>21</v>
       </c>
@@ -14042,9 +13751,9 @@
       <c r="T2" s="12"/>
       <c r="U2" s="12"/>
     </row>
-    <row r="3" spans="2:21" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:21" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -14083,28 +13792,28 @@
         <v>29</v>
       </c>
       <c r="O3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="T3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="U3" s="1" t="s">
-        <v>37</v>
-      </c>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B4" s="5">
         <v>0</v>
       </c>
@@ -14118,7 +13827,7 @@
         <v>110</v>
       </c>
       <c r="F4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -14142,7 +13851,7 @@
         <v>1</v>
       </c>
       <c r="N4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O4">
         <v>249.77337254090111</v>
@@ -14166,7 +13875,7 @@
         <v>62.685694944002243</v>
       </c>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B5" s="6">
         <v>0</v>
       </c>
@@ -14180,7 +13889,7 @@
         <v>230</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -14204,7 +13913,7 @@
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O5">
         <v>186.50014215467559</v>
@@ -14228,7 +13937,7 @@
         <v>4.6940612542763492E-4</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>0</v>
       </c>
@@ -14242,7 +13951,7 @@
         <v>230</v>
       </c>
       <c r="F6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -14266,7 +13975,7 @@
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O6">
         <v>-226.27351469557689</v>
@@ -14290,7 +13999,7 @@
         <v>5.7164316576912254E-4</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>0</v>
       </c>
@@ -14304,7 +14013,7 @@
         <v>230</v>
       </c>
       <c r="F7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -14328,7 +14037,7 @@
         <v>1</v>
       </c>
       <c r="N7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O7">
         <v>-51.993239722798748</v>
@@ -14352,7 +14061,7 @@
         <v>2.7251959471649522E-4</v>
       </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>0</v>
       </c>
@@ -14366,7 +14075,7 @@
         <v>230</v>
       </c>
       <c r="F8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G8">
         <v>2</v>
@@ -14390,7 +14099,7 @@
         <v>1</v>
       </c>
       <c r="N8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O8">
         <v>-28.62865718339954</v>
@@ -14414,7 +14123,7 @@
         <v>7.2340501901582756E-5</v>
       </c>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>0</v>
       </c>
@@ -14428,7 +14137,7 @@
         <v>230</v>
       </c>
       <c r="F9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G9">
         <v>3</v>
@@ -14452,7 +14161,7 @@
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O9">
         <v>-238.1886879666861</v>
@@ -14476,7 +14185,7 @@
         <v>100.17316388101121</v>
       </c>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B10">
         <f>B4+1</f>
         <v>1</v>
@@ -14491,7 +14200,7 @@
         <v>110</v>
       </c>
       <c r="F10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -14515,7 +14224,7 @@
         <v>1</v>
       </c>
       <c r="N10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O10">
         <v>249.77337254090111</v>
@@ -14541,7 +14250,7 @@
         <v>68.954264438402475</v>
       </c>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B11">
         <f>B5+1</f>
         <v>1</v>
@@ -14556,7 +14265,7 @@
         <v>230</v>
       </c>
       <c r="F11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -14580,7 +14289,7 @@
         <v>1</v>
       </c>
       <c r="N11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O11">
         <v>186.50014215467559</v>
@@ -14606,7 +14315,7 @@
         <v>5.1634673797039843E-4</v>
       </c>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B12">
         <f t="shared" ref="B12:B69" si="0">B6+1</f>
         <v>1</v>
@@ -14621,7 +14330,7 @@
         <v>230</v>
       </c>
       <c r="F12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -14645,7 +14354,7 @@
         <v>1</v>
       </c>
       <c r="N12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O12">
         <v>-226.27351469557689</v>
@@ -14671,7 +14380,7 @@
         <v>6.2880748234603486E-4</v>
       </c>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B13">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -14686,7 +14395,7 @@
         <v>230</v>
       </c>
       <c r="F13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -14710,7 +14419,7 @@
         <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O13">
         <v>-51.993239722798748</v>
@@ -14736,7 +14445,7 @@
         <v>2.9977155418814476E-4</v>
       </c>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B14">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -14751,7 +14460,7 @@
         <v>230</v>
       </c>
       <c r="F14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G14">
         <v>2</v>
@@ -14775,7 +14484,7 @@
         <v>1</v>
       </c>
       <c r="N14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O14">
         <v>-28.62865718339954</v>
@@ -14801,7 +14510,7 @@
         <v>7.9574552091741038E-5</v>
       </c>
     </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B15">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -14816,7 +14525,7 @@
         <v>230</v>
       </c>
       <c r="F15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G15">
         <v>3</v>
@@ -14840,7 +14549,7 @@
         <v>1</v>
       </c>
       <c r="N15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O15">
         <v>-238.1886879666861</v>
@@ -14866,7 +14575,7 @@
         <v>110.19048026911234</v>
       </c>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B16">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -14881,7 +14590,7 @@
         <v>110</v>
       </c>
       <c r="F16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -14905,7 +14614,7 @@
         <v>1</v>
       </c>
       <c r="N16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O16">
         <v>249.77337254090111</v>
@@ -14931,7 +14640,7 @@
         <v>75.849690882242726</v>
       </c>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B17">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -14946,7 +14655,7 @@
         <v>230</v>
       </c>
       <c r="F17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -14970,7 +14679,7 @@
         <v>1</v>
       </c>
       <c r="N17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O17">
         <v>186.50014215467559</v>
@@ -14996,7 +14705,7 @@
         <v>5.6798141176743835E-4</v>
       </c>
     </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B18">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -15011,7 +14720,7 @@
         <v>230</v>
       </c>
       <c r="F18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -15035,7 +14744,7 @@
         <v>1</v>
       </c>
       <c r="N18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O18">
         <v>-226.27351469557689</v>
@@ -15061,7 +14770,7 @@
         <v>6.9168823058063844E-4</v>
       </c>
     </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B19">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -15076,7 +14785,7 @@
         <v>230</v>
       </c>
       <c r="F19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -15100,7 +14809,7 @@
         <v>1</v>
       </c>
       <c r="N19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O19">
         <v>-51.993239722798748</v>
@@ -15126,7 +14835,7 @@
         <v>3.2974870960695928E-4</v>
       </c>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B20">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -15141,7 +14850,7 @@
         <v>230</v>
       </c>
       <c r="F20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G20">
         <v>2</v>
@@ -15165,7 +14874,7 @@
         <v>1</v>
       </c>
       <c r="N20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O20">
         <v>-28.62865718339954</v>
@@ -15191,7 +14900,7 @@
         <v>8.753200730091515E-5</v>
       </c>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B21">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -15206,7 +14915,7 @@
         <v>230</v>
       </c>
       <c r="F21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G21">
         <v>3</v>
@@ -15230,7 +14939,7 @@
         <v>1</v>
       </c>
       <c r="N21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O21">
         <v>-238.1886879666861</v>
@@ -15256,7 +14965,7 @@
         <v>121.20952829602359</v>
       </c>
     </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B22">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -15271,7 +14980,7 @@
         <v>110</v>
       </c>
       <c r="F22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -15295,7 +15004,7 @@
         <v>1</v>
       </c>
       <c r="N22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O22">
         <v>249.77337254090111</v>
@@ -15321,7 +15030,7 @@
         <v>83.43465997046701</v>
       </c>
     </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B23">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -15336,7 +15045,7 @@
         <v>230</v>
       </c>
       <c r="F23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -15360,7 +15069,7 @@
         <v>1</v>
       </c>
       <c r="N23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O23">
         <v>186.50014215467559</v>
@@ -15386,7 +15095,7 @@
         <v>6.247795529441822E-4</v>
       </c>
     </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B24">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -15401,7 +15110,7 @@
         <v>230</v>
       </c>
       <c r="F24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -15425,7 +15134,7 @@
         <v>1</v>
       </c>
       <c r="N24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O24">
         <v>-226.27351469557689</v>
@@ -15451,7 +15160,7 @@
         <v>7.608570536387023E-4</v>
       </c>
     </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B25">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -15466,7 +15175,7 @@
         <v>230</v>
       </c>
       <c r="F25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -15490,7 +15199,7 @@
         <v>1</v>
       </c>
       <c r="N25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O25">
         <v>-51.993239722798748</v>
@@ -15516,7 +15225,7 @@
         <v>3.6272358056765522E-4</v>
       </c>
     </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B26">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -15531,7 +15240,7 @@
         <v>230</v>
       </c>
       <c r="F26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G26">
         <v>2</v>
@@ -15555,7 +15264,7 @@
         <v>1</v>
       </c>
       <c r="N26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O26">
         <v>-28.62865718339954</v>
@@ -15581,7 +15290,7 @@
         <v>9.6285208031006677E-5</v>
       </c>
     </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B27">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -15596,7 +15305,7 @@
         <v>230</v>
       </c>
       <c r="F27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G27">
         <v>3</v>
@@ -15620,7 +15329,7 @@
         <v>1</v>
       </c>
       <c r="N27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O27">
         <v>-238.1886879666861</v>
@@ -15646,7 +15355,7 @@
         <v>133.33048112562597</v>
       </c>
     </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B28">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -15661,7 +15370,7 @@
         <v>110</v>
       </c>
       <c r="F28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -15685,7 +15394,7 @@
         <v>1</v>
       </c>
       <c r="N28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O28">
         <v>249.77337254090111</v>
@@ -15711,7 +15420,7 @@
         <v>91.778125967513716</v>
       </c>
     </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B29">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -15726,7 +15435,7 @@
         <v>230</v>
       </c>
       <c r="F29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -15750,7 +15459,7 @@
         <v>1</v>
       </c>
       <c r="N29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O29">
         <v>186.50014215467559</v>
@@ -15776,7 +15485,7 @@
         <v>6.8725750823860044E-4</v>
       </c>
     </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B30">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -15791,7 +15500,7 @@
         <v>230</v>
       </c>
       <c r="F30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -15815,7 +15524,7 @@
         <v>1</v>
       </c>
       <c r="N30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O30">
         <v>-226.27351469557689</v>
@@ -15841,7 +15550,7 @@
         <v>8.3694275900257262E-4</v>
       </c>
     </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B31">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -15856,7 +15565,7 @@
         <v>230</v>
       </c>
       <c r="F31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G31">
         <v>1</v>
@@ -15880,7 +15589,7 @@
         <v>1</v>
       </c>
       <c r="N31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O31">
         <v>-51.993239722798748</v>
@@ -15906,7 +15615,7 @@
         <v>3.9899593862442078E-4</v>
       </c>
     </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B32">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -15921,7 +15630,7 @@
         <v>230</v>
       </c>
       <c r="F32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G32">
         <v>2</v>
@@ -15945,7 +15654,7 @@
         <v>1</v>
       </c>
       <c r="N32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O32">
         <v>-28.62865718339954</v>
@@ -15971,7 +15680,7 @@
         <v>1.0591372883410735E-4</v>
       </c>
     </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B33">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -15986,7 +15695,7 @@
         <v>230</v>
       </c>
       <c r="F33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G33">
         <v>3</v>
@@ -16010,7 +15719,7 @@
         <v>1</v>
       </c>
       <c r="N33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O33">
         <v>-238.1886879666861</v>
@@ -16036,7 +15745,7 @@
         <v>146.66352923818857</v>
       </c>
     </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B34">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -16051,7 +15760,7 @@
         <v>110</v>
       </c>
       <c r="F34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -16075,7 +15784,7 @@
         <v>1</v>
       </c>
       <c r="N34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O34">
         <v>249.77337254090111</v>
@@ -16101,7 +15810,7 @@
         <v>100.9559385642651</v>
       </c>
     </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B35">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -16116,7 +15825,7 @@
         <v>230</v>
       </c>
       <c r="F35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -16140,7 +15849,7 @@
         <v>1</v>
       </c>
       <c r="N35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O35">
         <v>186.50014215467559</v>
@@ -16166,7 +15875,7 @@
         <v>7.559832590624605E-4</v>
       </c>
     </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B36">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -16181,7 +15890,7 @@
         <v>230</v>
       </c>
       <c r="F36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -16205,7 +15914,7 @@
         <v>1</v>
       </c>
       <c r="N36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O36">
         <v>-226.27351469557689</v>
@@ -16231,7 +15940,7 @@
         <v>9.2063703490282995E-4</v>
       </c>
     </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B37">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -16246,7 +15955,7 @@
         <v>230</v>
       </c>
       <c r="F37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G37">
         <v>1</v>
@@ -16270,7 +15979,7 @@
         <v>1</v>
       </c>
       <c r="N37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O37">
         <v>-51.993239722798748</v>
@@ -16296,7 +16005,7 @@
         <v>4.3889553248686289E-4</v>
       </c>
     </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B38">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -16311,7 +16020,7 @@
         <v>230</v>
       </c>
       <c r="F38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G38">
         <v>2</v>
@@ -16335,7 +16044,7 @@
         <v>1</v>
       </c>
       <c r="N38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O38">
         <v>-28.62865718339954</v>
@@ -16361,7 +16070,7 @@
         <v>1.165051017175181E-4</v>
       </c>
     </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B39">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -16376,7 +16085,7 @@
         <v>230</v>
       </c>
       <c r="F39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G39">
         <v>3</v>
@@ -16400,7 +16109,7 @@
         <v>1</v>
       </c>
       <c r="N39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O39">
         <v>-238.1886879666861</v>
@@ -16426,7 +16135,7 @@
         <v>161.32988216200744</v>
       </c>
     </row>
-    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B40">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -16441,7 +16150,7 @@
         <v>110</v>
       </c>
       <c r="F40" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -16465,7 +16174,7 @@
         <v>1</v>
       </c>
       <c r="N40" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O40">
         <v>249.77337254090111</v>
@@ -16491,7 +16200,7 @@
         <v>111.05153242069161</v>
       </c>
     </row>
-    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B41">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -16506,7 +16215,7 @@
         <v>230</v>
       </c>
       <c r="F41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -16530,7 +16239,7 @@
         <v>1</v>
       </c>
       <c r="N41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O41">
         <v>186.50014215467559</v>
@@ -16556,7 +16265,7 @@
         <v>8.3158158496870658E-4</v>
       </c>
     </row>
-    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B42">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -16571,7 +16280,7 @@
         <v>230</v>
       </c>
       <c r="F42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -16595,7 +16304,7 @@
         <v>1</v>
       </c>
       <c r="N42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O42">
         <v>-226.27351469557689</v>
@@ -16621,7 +16330,7 @@
         <v>1.012700738393113E-3</v>
       </c>
     </row>
-    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B43">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -16636,7 +16345,7 @@
         <v>230</v>
       </c>
       <c r="F43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G43">
         <v>1</v>
@@ -16660,7 +16369,7 @@
         <v>1</v>
       </c>
       <c r="N43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O43">
         <v>-51.993239722798748</v>
@@ -16686,7 +16395,7 @@
         <v>4.827850857355492E-4</v>
       </c>
     </row>
-    <row r="44" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B44">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -16701,7 +16410,7 @@
         <v>230</v>
       </c>
       <c r="F44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G44">
         <v>2</v>
@@ -16725,7 +16434,7 @@
         <v>1</v>
       </c>
       <c r="N44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O44">
         <v>-28.62865718339954</v>
@@ -16751,7 +16460,7 @@
         <v>1.2815561188926991E-4</v>
       </c>
     </row>
-    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B45">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -16766,7 +16475,7 @@
         <v>230</v>
       </c>
       <c r="F45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G45">
         <v>3</v>
@@ -16790,7 +16499,7 @@
         <v>1</v>
       </c>
       <c r="N45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O45">
         <v>-238.1886879666861</v>
@@ -16816,7 +16525,7 @@
         <v>177.46287037820821</v>
       </c>
     </row>
-    <row r="46" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B46">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -16831,7 +16540,7 @@
         <v>110</v>
       </c>
       <c r="F46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -16855,7 +16564,7 @@
         <v>1</v>
       </c>
       <c r="N46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O46">
         <v>249.77337254090111</v>
@@ -16881,7 +16590,7 @@
         <v>122.15668566276078</v>
       </c>
     </row>
-    <row r="47" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B47">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -16896,7 +16605,7 @@
         <v>230</v>
       </c>
       <c r="F47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -16920,7 +16629,7 @@
         <v>1</v>
       </c>
       <c r="N47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O47">
         <v>186.50014215467559</v>
@@ -16946,7 +16655,7 @@
         <v>9.1473974346557732E-4</v>
       </c>
     </row>
-    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B48">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -16961,7 +16670,7 @@
         <v>230</v>
       </c>
       <c r="F48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -16985,7 +16694,7 @@
         <v>1</v>
       </c>
       <c r="N48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O48">
         <v>-226.27351469557689</v>
@@ -17011,7 +16720,7 @@
         <v>1.1139708122324245E-3</v>
       </c>
     </row>
-    <row r="49" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B49">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -17026,7 +16735,7 @@
         <v>230</v>
       </c>
       <c r="F49" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G49">
         <v>1</v>
@@ -17050,7 +16759,7 @@
         <v>1</v>
       </c>
       <c r="N49" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O49">
         <v>-51.993239722798748</v>
@@ -17076,7 +16785,7 @@
         <v>5.3106359430910412E-4</v>
       </c>
     </row>
-    <row r="50" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B50">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -17091,7 +16800,7 @@
         <v>230</v>
       </c>
       <c r="F50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G50">
         <v>2</v>
@@ -17115,7 +16824,7 @@
         <v>1</v>
       </c>
       <c r="N50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O50">
         <v>-28.62865718339954</v>
@@ -17141,7 +16850,7 @@
         <v>1.4097117307819692E-4</v>
       </c>
     </row>
-    <row r="51" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B51">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -17156,7 +16865,7 @@
         <v>230</v>
       </c>
       <c r="F51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G51">
         <v>3</v>
@@ -17180,7 +16889,7 @@
         <v>1</v>
       </c>
       <c r="N51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O51">
         <v>-238.1886879666861</v>
@@ -17206,7 +16915,7 @@
         <v>195.20915741602906</v>
       </c>
     </row>
-    <row r="52" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B52">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -17221,7 +16930,7 @@
         <v>110</v>
       </c>
       <c r="F52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G52">
         <v>0</v>
@@ -17245,7 +16954,7 @@
         <v>1</v>
       </c>
       <c r="N52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O52">
         <v>-447.74871874997302</v>
@@ -17271,7 +16980,7 @@
         <v>134.37235422903686</v>
       </c>
     </row>
-    <row r="53" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B53">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -17286,7 +16995,7 @@
         <v>230</v>
       </c>
       <c r="F53" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -17310,7 +17019,7 @@
         <v>1</v>
       </c>
       <c r="N53" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O53">
         <v>-657.30874953325997</v>
@@ -17336,7 +17045,7 @@
         <v>1.0062137178121352E-3</v>
       </c>
     </row>
-    <row r="54" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B54">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -17351,7 +17060,7 @@
         <v>230</v>
       </c>
       <c r="F54" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -17375,7 +17084,7 @@
         <v>1</v>
       </c>
       <c r="N54" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O54">
         <v>-866.86878031654601</v>
@@ -17401,7 +17110,7 @@
         <v>1.2253678934556671E-3</v>
       </c>
     </row>
-    <row r="55" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B55">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -17416,7 +17125,7 @@
         <v>230</v>
       </c>
       <c r="F55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G55">
         <v>1</v>
@@ -17440,7 +17149,7 @@
         <v>1</v>
       </c>
       <c r="N55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O55">
         <v>-1076.42881109983</v>
@@ -17466,7 +17175,7 @@
         <v>5.8416995374001453E-4</v>
       </c>
     </row>
-    <row r="56" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B56">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -17481,7 +17190,7 @@
         <v>230</v>
       </c>
       <c r="F56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G56">
         <v>2</v>
@@ -17505,7 +17214,7 @@
         <v>1</v>
       </c>
       <c r="N56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O56">
         <v>-1285.9888418831199</v>
@@ -17531,7 +17240,7 @@
         <v>1.5506829038601662E-4</v>
       </c>
     </row>
-    <row r="57" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B57">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -17546,7 +17255,7 @@
         <v>230</v>
       </c>
       <c r="F57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G57">
         <v>3</v>
@@ -17570,7 +17279,7 @@
         <v>1</v>
       </c>
       <c r="N57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O57">
         <v>-1495.54887266641</v>
@@ -17596,7 +17305,7 @@
         <v>214.73007315763198</v>
       </c>
     </row>
-    <row r="58" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B58">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -17611,7 +17320,7 @@
         <v>110</v>
       </c>
       <c r="F58" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -17635,7 +17344,7 @@
         <v>1</v>
       </c>
       <c r="N58" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O58">
         <v>-1705.1089034496899</v>
@@ -17661,7 +17370,7 @@
         <v>147.80958965194057</v>
       </c>
     </row>
-    <row r="59" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B59">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -17676,7 +17385,7 @@
         <v>230</v>
       </c>
       <c r="F59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -17700,7 +17409,7 @@
         <v>1</v>
       </c>
       <c r="N59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O59">
         <v>-1914.6689342329801</v>
@@ -17726,7 +17435,7 @@
         <v>1.1068350895933488E-3</v>
       </c>
     </row>
-    <row r="60" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B60">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -17741,7 +17450,7 @@
         <v>230</v>
       </c>
       <c r="F60" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -17765,7 +17474,7 @@
         <v>1</v>
       </c>
       <c r="N60" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O60">
         <v>-2124.2289650162702</v>
@@ -17791,7 +17500,7 @@
         <v>1.347904682801234E-3</v>
       </c>
     </row>
-    <row r="61" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B61">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -17806,7 +17515,7 @@
         <v>230</v>
       </c>
       <c r="F61" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G61">
         <v>1</v>
@@ -17830,7 +17539,7 @@
         <v>1</v>
       </c>
       <c r="N61" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O61">
         <v>-2333.7889957995499</v>
@@ -17856,7 +17565,7 @@
         <v>6.4258694911401601E-4</v>
       </c>
     </row>
-    <row r="62" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B62">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -17871,7 +17580,7 @@
         <v>230</v>
       </c>
       <c r="F62" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G62">
         <v>2</v>
@@ -17895,7 +17604,7 @@
         <v>1</v>
       </c>
       <c r="N62" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O62">
         <v>-2543.34902658284</v>
@@ -17921,7 +17630,7 @@
         <v>1.7057511942461829E-4</v>
       </c>
     </row>
-    <row r="63" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B63">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -17936,7 +17645,7 @@
         <v>230</v>
       </c>
       <c r="F63" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G63">
         <v>3</v>
@@ -17960,7 +17669,7 @@
         <v>1</v>
       </c>
       <c r="N63" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O63">
         <v>-2752.9090573661301</v>
@@ -17986,7 +17695,7 @@
         <v>236.2030804733952</v>
       </c>
     </row>
-    <row r="64" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B64">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -18001,7 +17710,7 @@
         <v>110</v>
       </c>
       <c r="F64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G64">
         <v>0</v>
@@ -18025,7 +17734,7 @@
         <v>1</v>
       </c>
       <c r="N64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O64">
         <v>-2962.4690881494098</v>
@@ -18051,7 +17760,7 @@
         <v>162.59054861713463</v>
       </c>
     </row>
-    <row r="65" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B65">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -18066,7 +17775,7 @@
         <v>230</v>
       </c>
       <c r="F65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -18090,7 +17799,7 @@
         <v>1</v>
       </c>
       <c r="N65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O65">
         <v>-3172.0291189326999</v>
@@ -18116,7 +17825,7 @@
         <v>1.2175185985526839E-3</v>
       </c>
     </row>
-    <row r="66" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B66">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -18131,7 +17840,7 @@
         <v>230</v>
       </c>
       <c r="F66" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G66">
         <v>0</v>
@@ -18155,7 +17864,7 @@
         <v>1</v>
       </c>
       <c r="N66" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O66">
         <v>-3381.5891497159801</v>
@@ -18181,7 +17890,7 @@
         <v>1.4826951510813575E-3</v>
       </c>
     </row>
-    <row r="67" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B67">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -18196,7 +17905,7 @@
         <v>230</v>
       </c>
       <c r="F67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G67">
         <v>1</v>
@@ -18220,7 +17929,7 @@
         <v>1</v>
       </c>
       <c r="N67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O67">
         <v>-3591.1491804992702</v>
@@ -18246,7 +17955,7 @@
         <v>7.0684564402541763E-4</v>
       </c>
     </row>
-    <row r="68" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B68">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -18261,7 +17970,7 @@
         <v>230</v>
       </c>
       <c r="F68" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G68">
         <v>2</v>
@@ -18285,7 +17994,7 @@
         <v>1</v>
       </c>
       <c r="N68" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O68">
         <v>-3800.7092112825599</v>
@@ -18311,7 +18020,7 @@
         <v>1.8763263136708014E-4</v>
       </c>
     </row>
-    <row r="69" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B69">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -18326,7 +18035,7 @@
         <v>230</v>
       </c>
       <c r="F69" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G69">
         <v>3</v>
@@ -18350,7 +18059,7 @@
         <v>1</v>
       </c>
       <c r="N69" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O69">
         <v>-4010.26924206584</v>
@@ -18392,20 +18101,20 @@
   <dimension ref="B2:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:22" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:22" ht="21" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
@@ -18428,79 +18137,200 @@
       <c r="U2" s="12"/>
       <c r="V2" s="12"/>
     </row>
-    <row r="3" spans="2:22" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:22" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="P3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="S3" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="T3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U3" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="U3" s="7" t="s">
+      <c r="V3" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="V3" s="7" t="s">
-        <v>37</v>
-      </c>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B4" s="5"/>
-      <c r="N4" t="s">
-        <v>30</v>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4">
+        <v>0.4</v>
+      </c>
+      <c r="K4">
+        <v>0.6</v>
+      </c>
+      <c r="L4">
+        <v>150</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>0.1236666454897191</v>
+      </c>
+      <c r="Q4">
+        <v>4.3409192649510153E-2</v>
+      </c>
+      <c r="R4">
+        <v>-0.1222531233879495</v>
+      </c>
+      <c r="S4">
+        <v>-4.0798601062843547E-2</v>
+      </c>
+      <c r="T4">
+        <v>1.413522101769524E-3</v>
+      </c>
+      <c r="U4">
+        <v>2.6105915866666001E-3</v>
+      </c>
+      <c r="V4">
+        <v>52.425638328073241</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B5" s="6">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>0.4</v>
+      </c>
+      <c r="K5">
+        <v>0.6</v>
+      </c>
+      <c r="L5">
+        <v>150</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>0.1236666454897191</v>
+      </c>
+      <c r="Q5">
+        <v>4.3409192649510153E-2</v>
+      </c>
+      <c r="R5">
+        <v>-0.1222531233879495</v>
+      </c>
+      <c r="S5">
+        <v>-4.0798601062843547E-2</v>
+      </c>
+      <c r="T5">
+        <v>1.413522101769524E-3</v>
+      </c>
+      <c r="U5">
+        <v>2.6105915866666001E-3</v>
+      </c>
+      <c r="V5">
+        <v>52.425638328073241</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -18518,17 +18348,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0615AB1B-76EC-4323-8F51-232F31293F22}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q49" sqref="Q49"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" customWidth="1"/>
+    <col min="1" max="1" width="1.5546875" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -18547,21 +18377,21 @@
   <dimension ref="B2:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" ht="21" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
         <v>10</v>
       </c>
@@ -18573,9 +18403,9 @@
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
     </row>
-    <row r="3" spans="2:9" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -18599,10 +18429,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="5"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="6"/>
     </row>
   </sheetData>
@@ -18625,26 +18455,26 @@
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
-    <col min="14" max="15" width="14.85546875" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="13" max="13" width="14.109375" customWidth="1"/>
+    <col min="14" max="15" width="14.88671875" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:17" ht="21" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
@@ -18662,9 +18492,9 @@
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
     </row>
-    <row r="3" spans="2:17" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:17" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -18676,10 +18506,10 @@
         <v>18</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>6</v>
@@ -18712,7 +18542,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B4" s="5">
         <v>0</v>
       </c>
@@ -18726,16 +18556,16 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" t="s">
         <v>61</v>
-      </c>
-      <c r="G4" t="s">
-        <v>62</v>
       </c>
       <c r="H4">
         <v>230</v>
       </c>
       <c r="I4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -18762,7 +18592,7 @@
         <v>30.72515988161237</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="6">
         <v>0</v>
       </c>
@@ -18776,16 +18606,16 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" t="s">
         <v>64</v>
-      </c>
-      <c r="G5" t="s">
-        <v>65</v>
       </c>
       <c r="H5">
         <v>230</v>
       </c>
       <c r="I5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -18812,7 +18642,7 @@
         <v>194.6547201924518</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>0</v>
       </c>
@@ -18826,16 +18656,16 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" t="s">
         <v>66</v>
-      </c>
-      <c r="G6" t="s">
-        <v>67</v>
       </c>
       <c r="H6">
         <v>110</v>
       </c>
       <c r="I6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -18862,7 +18692,7 @@
         <v>-38.209623444425397</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>1</v>
       </c>
@@ -18876,16 +18706,16 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" t="s">
         <v>61</v>
-      </c>
-      <c r="G7" t="s">
-        <v>62</v>
       </c>
       <c r="H7">
         <v>230</v>
       </c>
       <c r="I7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -18913,7 +18743,7 @@
         <v>30.72515988161237</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>1</v>
       </c>
@@ -18927,16 +18757,16 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" t="s">
         <v>64</v>
-      </c>
-      <c r="G8" t="s">
-        <v>65</v>
       </c>
       <c r="H8">
         <v>230</v>
       </c>
       <c r="I8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -18964,7 +18794,7 @@
         <v>194.6547201924518</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>1</v>
       </c>
@@ -18978,16 +18808,16 @@
         <v>2</v>
       </c>
       <c r="F9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" t="s">
         <v>66</v>
-      </c>
-      <c r="G9" t="s">
-        <v>67</v>
       </c>
       <c r="H9">
         <v>110</v>
       </c>
       <c r="I9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -19015,7 +18845,7 @@
         <v>-38.209623444425397</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>2</v>
       </c>
@@ -19029,16 +18859,16 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" t="s">
         <v>61</v>
-      </c>
-      <c r="G10" t="s">
-        <v>62</v>
       </c>
       <c r="H10">
         <v>230</v>
       </c>
       <c r="I10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -19071,7 +18901,7 @@
         <v>33.797675869773613</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>2</v>
       </c>
@@ -19085,16 +18915,16 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" t="s">
         <v>64</v>
-      </c>
-      <c r="G11" t="s">
-        <v>65</v>
       </c>
       <c r="H11">
         <v>230</v>
       </c>
       <c r="I11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -19127,7 +18957,7 @@
         <v>214.120192211697</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>2</v>
       </c>
@@ -19141,16 +18971,16 @@
         <v>2</v>
       </c>
       <c r="F12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" t="s">
         <v>66</v>
-      </c>
-      <c r="G12" t="s">
-        <v>67</v>
       </c>
       <c r="H12">
         <v>110</v>
       </c>
       <c r="I12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J12">
         <v>1</v>
@@ -19183,7 +19013,7 @@
         <v>-42.030585788867938</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>3</v>
       </c>
@@ -19197,16 +19027,16 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" t="s">
         <v>61</v>
-      </c>
-      <c r="G13" t="s">
-        <v>62</v>
       </c>
       <c r="H13">
         <v>230</v>
       </c>
       <c r="I13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -19239,7 +19069,7 @@
         <v>33.797675869773613</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>3</v>
       </c>
@@ -19253,16 +19083,16 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" t="s">
         <v>64</v>
-      </c>
-      <c r="G14" t="s">
-        <v>65</v>
       </c>
       <c r="H14">
         <v>230</v>
       </c>
       <c r="I14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -19295,7 +19125,7 @@
         <v>214.120192211697</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>3</v>
       </c>
@@ -19309,16 +19139,16 @@
         <v>2</v>
       </c>
       <c r="F15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" t="s">
         <v>66</v>
-      </c>
-      <c r="G15" t="s">
-        <v>67</v>
       </c>
       <c r="H15">
         <v>110</v>
       </c>
       <c r="I15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J15">
         <v>1</v>
@@ -19351,7 +19181,7 @@
         <v>-42.030585788867938</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>4</v>
       </c>
@@ -19365,16 +19195,16 @@
         <v>0</v>
       </c>
       <c r="F16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" t="s">
         <v>61</v>
-      </c>
-      <c r="G16" t="s">
-        <v>62</v>
       </c>
       <c r="H16">
         <v>230</v>
       </c>
       <c r="I16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J16">
         <v>1</v>
@@ -19407,7 +19237,7 @@
         <v>37.177443456750979</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>4</v>
       </c>
@@ -19421,16 +19251,16 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" t="s">
         <v>64</v>
-      </c>
-      <c r="G17" t="s">
-        <v>65</v>
       </c>
       <c r="H17">
         <v>230</v>
       </c>
       <c r="I17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J17">
         <v>1</v>
@@ -19463,7 +19293,7 @@
         <v>235.53221143286672</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>4</v>
       </c>
@@ -19477,16 +19307,16 @@
         <v>2</v>
       </c>
       <c r="F18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" t="s">
         <v>66</v>
-      </c>
-      <c r="G18" t="s">
-        <v>67</v>
       </c>
       <c r="H18">
         <v>110</v>
       </c>
       <c r="I18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J18">
         <v>1</v>
@@ -19519,7 +19349,7 @@
         <v>-46.233644367754735</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>5</v>
       </c>
@@ -19533,16 +19363,16 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" t="s">
         <v>61</v>
-      </c>
-      <c r="G19" t="s">
-        <v>62</v>
       </c>
       <c r="H19">
         <v>230</v>
       </c>
       <c r="I19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J19">
         <v>1</v>
@@ -19575,7 +19405,7 @@
         <v>37.177443456750979</v>
       </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>5</v>
       </c>
@@ -19589,16 +19419,16 @@
         <v>1</v>
       </c>
       <c r="F20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" t="s">
         <v>64</v>
-      </c>
-      <c r="G20" t="s">
-        <v>65</v>
       </c>
       <c r="H20">
         <v>230</v>
       </c>
       <c r="I20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J20">
         <v>1</v>
@@ -19631,7 +19461,7 @@
         <v>235.53221143286672</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>5</v>
       </c>
@@ -19645,16 +19475,16 @@
         <v>2</v>
       </c>
       <c r="F21" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" t="s">
         <v>66</v>
-      </c>
-      <c r="G21" t="s">
-        <v>67</v>
       </c>
       <c r="H21">
         <v>110</v>
       </c>
       <c r="I21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J21">
         <v>1</v>
@@ -19687,7 +19517,7 @@
         <v>-46.233644367754735</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>6</v>
       </c>
@@ -19701,16 +19531,16 @@
         <v>0</v>
       </c>
       <c r="F22" t="s">
+        <v>60</v>
+      </c>
+      <c r="G22" t="s">
         <v>61</v>
-      </c>
-      <c r="G22" t="s">
-        <v>62</v>
       </c>
       <c r="H22">
         <v>230</v>
       </c>
       <c r="I22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J22">
         <v>1</v>
@@ -19743,7 +19573,7 @@
         <v>40.895187802426079</v>
       </c>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>6</v>
       </c>
@@ -19757,16 +19587,16 @@
         <v>1</v>
       </c>
       <c r="F23" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23" t="s">
         <v>64</v>
-      </c>
-      <c r="G23" t="s">
-        <v>65</v>
       </c>
       <c r="H23">
         <v>230</v>
       </c>
       <c r="I23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J23">
         <v>1</v>
@@ -19799,7 +19629,7 @@
         <v>259.08543257615344</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>6</v>
       </c>
@@ -19813,16 +19643,16 @@
         <v>2</v>
       </c>
       <c r="F24" t="s">
+        <v>65</v>
+      </c>
+      <c r="G24" t="s">
         <v>66</v>
-      </c>
-      <c r="G24" t="s">
-        <v>67</v>
       </c>
       <c r="H24">
         <v>110</v>
       </c>
       <c r="I24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J24">
         <v>1</v>
@@ -19855,7 +19685,7 @@
         <v>-50.85700880453021</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>7</v>
       </c>
@@ -19869,16 +19699,16 @@
         <v>0</v>
       </c>
       <c r="F25" t="s">
+        <v>60</v>
+      </c>
+      <c r="G25" t="s">
         <v>61</v>
-      </c>
-      <c r="G25" t="s">
-        <v>62</v>
       </c>
       <c r="H25">
         <v>230</v>
       </c>
       <c r="I25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J25">
         <v>1</v>
@@ -19911,7 +19741,7 @@
         <v>40.895187802426079</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>7</v>
       </c>
@@ -19925,16 +19755,16 @@
         <v>1</v>
       </c>
       <c r="F26" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26" t="s">
         <v>64</v>
-      </c>
-      <c r="G26" t="s">
-        <v>65</v>
       </c>
       <c r="H26">
         <v>230</v>
       </c>
       <c r="I26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J26">
         <v>1</v>
@@ -19967,7 +19797,7 @@
         <v>259.08543257615344</v>
       </c>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>7</v>
       </c>
@@ -19981,16 +19811,16 @@
         <v>2</v>
       </c>
       <c r="F27" t="s">
+        <v>65</v>
+      </c>
+      <c r="G27" t="s">
         <v>66</v>
-      </c>
-      <c r="G27" t="s">
-        <v>67</v>
       </c>
       <c r="H27">
         <v>110</v>
       </c>
       <c r="I27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J27">
         <v>1</v>
@@ -20023,7 +19853,7 @@
         <v>-50.85700880453021</v>
       </c>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>8</v>
       </c>
@@ -20037,16 +19867,16 @@
         <v>0</v>
       </c>
       <c r="F28" t="s">
+        <v>60</v>
+      </c>
+      <c r="G28" t="s">
         <v>61</v>
-      </c>
-      <c r="G28" t="s">
-        <v>62</v>
       </c>
       <c r="H28">
         <v>230</v>
       </c>
       <c r="I28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J28">
         <v>1</v>
@@ -20079,7 +19909,7 @@
         <v>44.984706582668693</v>
       </c>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>8</v>
       </c>
@@ -20093,16 +19923,16 @@
         <v>1</v>
       </c>
       <c r="F29" t="s">
+        <v>63</v>
+      </c>
+      <c r="G29" t="s">
         <v>64</v>
-      </c>
-      <c r="G29" t="s">
-        <v>65</v>
       </c>
       <c r="H29">
         <v>230</v>
       </c>
       <c r="I29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J29">
         <v>1</v>
@@ -20135,7 +19965,7 @@
         <v>284.99397583376879</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>8</v>
       </c>
@@ -20149,16 +19979,16 @@
         <v>2</v>
       </c>
       <c r="F30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G30" t="s">
         <v>66</v>
-      </c>
-      <c r="G30" t="s">
-        <v>67</v>
       </c>
       <c r="H30">
         <v>110</v>
       </c>
       <c r="I30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J30">
         <v>1</v>
@@ -20191,7 +20021,7 @@
         <v>-55.942709684983235</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>9</v>
       </c>
@@ -20205,16 +20035,16 @@
         <v>0</v>
       </c>
       <c r="F31" t="s">
+        <v>60</v>
+      </c>
+      <c r="G31" t="s">
         <v>61</v>
-      </c>
-      <c r="G31" t="s">
-        <v>62</v>
       </c>
       <c r="H31">
         <v>230</v>
       </c>
       <c r="I31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J31">
         <v>1</v>
@@ -20247,7 +20077,7 @@
         <v>44.984706582668693</v>
       </c>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>9</v>
       </c>
@@ -20261,16 +20091,16 @@
         <v>1</v>
       </c>
       <c r="F32" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" t="s">
         <v>64</v>
-      </c>
-      <c r="G32" t="s">
-        <v>65</v>
       </c>
       <c r="H32">
         <v>230</v>
       </c>
       <c r="I32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J32">
         <v>1</v>
@@ -20303,7 +20133,7 @@
         <v>284.99397583376879</v>
       </c>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>9</v>
       </c>
@@ -20317,16 +20147,16 @@
         <v>2</v>
       </c>
       <c r="F33" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" t="s">
         <v>66</v>
-      </c>
-      <c r="G33" t="s">
-        <v>67</v>
       </c>
       <c r="H33">
         <v>110</v>
       </c>
       <c r="I33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J33">
         <v>1</v>
@@ -20359,7 +20189,7 @@
         <v>-55.942709684983235</v>
       </c>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>10</v>
       </c>
@@ -20373,16 +20203,16 @@
         <v>0</v>
       </c>
       <c r="F34" t="s">
+        <v>60</v>
+      </c>
+      <c r="G34" t="s">
         <v>61</v>
-      </c>
-      <c r="G34" t="s">
-        <v>62</v>
       </c>
       <c r="H34">
         <v>230</v>
       </c>
       <c r="I34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J34">
         <v>1</v>
@@ -20415,7 +20245,7 @@
         <v>49.483177240935568</v>
       </c>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>10</v>
       </c>
@@ -20429,16 +20259,16 @@
         <v>1</v>
       </c>
       <c r="F35" t="s">
+        <v>63</v>
+      </c>
+      <c r="G35" t="s">
         <v>64</v>
-      </c>
-      <c r="G35" t="s">
-        <v>65</v>
       </c>
       <c r="H35">
         <v>230</v>
       </c>
       <c r="I35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J35">
         <v>1</v>
@@ -20471,7 +20301,7 @@
         <v>313.49337341714568</v>
       </c>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>10</v>
       </c>
@@ -20485,16 +20315,16 @@
         <v>2</v>
       </c>
       <c r="F36" t="s">
+        <v>65</v>
+      </c>
+      <c r="G36" t="s">
         <v>66</v>
-      </c>
-      <c r="G36" t="s">
-        <v>67</v>
       </c>
       <c r="H36">
         <v>110</v>
       </c>
       <c r="I36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J36">
         <v>1</v>
@@ -20546,386 +20376,386 @@
       <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="8" t="s">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" t="s">
         <v>69</v>
       </c>
+      <c r="D7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
         <v>61</v>
       </c>
-      <c r="C7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>64</v>
       </c>
-      <c r="E7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="F8" t="s">
         <v>66</v>
       </c>
-      <c r="G7" t="s">
-        <v>72</v>
-      </c>
-      <c r="H7" t="s">
-        <v>60</v>
-      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>0</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="13">
         <v>40</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="13">
         <v>40</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="13">
         <v>323.49</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="13">
         <v>323.49</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="13">
         <v>466.51</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="13">
         <v>466.51</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="13">
         <v>830</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>1</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="13">
         <v>44</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="13">
         <v>44</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="13">
         <v>355.83900000000006</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="13">
         <v>355.83900000000006</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="13">
         <v>513.16100000000006</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="13">
         <v>513.16100000000006</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="13">
         <v>913.00000000000011</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>2</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="13">
         <v>48.400000000000006</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="13">
         <v>48.400000000000006</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="13">
         <v>391.42290000000008</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="13">
         <v>391.42290000000008</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="13">
         <v>564.47710000000006</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="13">
         <v>564.47710000000006</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="13">
         <v>1004.3000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>3</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="13">
         <v>53.240000000000009</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="13">
         <v>53.240000000000009</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="13">
         <v>430.56519000000014</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="13">
         <v>430.56519000000014</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="13">
         <v>620.92481000000009</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="13">
         <v>620.92481000000009</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="13">
         <v>1104.7300000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>4</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="13">
         <v>58.564000000000014</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="13">
         <v>58.564000000000014</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="13">
         <v>473.62170900000018</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="13">
         <v>473.62170900000018</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="13">
         <v>683.01729100000011</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="13">
         <v>683.01729100000011</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="13">
         <v>1215.2030000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>5</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="13">
         <v>64.420400000000015</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="13">
         <v>64.420400000000015</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="13">
         <v>520.98387990000026</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="13">
         <v>520.98387990000026</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="13">
         <v>751.31902010000022</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="13">
         <v>751.31902010000022</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="13">
         <v>1336.7233000000006</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>6</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="13">
         <v>70.862440000000021</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="13">
         <v>70.862440000000021</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="13">
         <v>573.08226789000037</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="13">
         <v>573.08226789000037</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="13">
         <v>826.45092211000031</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="13">
         <v>826.45092211000031</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="13">
         <v>1470.3956300000007</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>7</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="13">
         <v>77.948684000000029</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="13">
         <v>77.948684000000029</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="13">
         <v>630.39049467900043</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="13">
         <v>630.39049467900043</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="13">
         <v>909.09601432100044</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="13">
         <v>909.09601432100044</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="13">
         <v>1617.4351930000009</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>8</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="13">
         <v>85.743552400000041</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="13">
         <v>85.743552400000041</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="13">
         <v>693.42954414690053</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="13">
         <v>693.42954414690053</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="13">
         <v>1000.0056157531005</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="13">
         <v>1000.0056157531005</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="13">
         <v>1779.1787123000011</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <v>9</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="13">
         <v>94.317907640000058</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="13">
         <v>94.317907640000058</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="13">
         <v>762.77249856159062</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="13">
         <v>762.77249856159062</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="13">
         <v>1100.0061773284106</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="13">
         <v>1100.0061773284106</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="13">
         <v>1957.0965835300012</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <v>10</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="13">
         <v>103.74969840400007</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="13">
         <v>103.74969840400007</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="13">
         <v>839.0497484177497</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="13">
         <v>839.0497484177497</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="13">
         <v>1210.0067950612518</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="13">
         <v>1210.0067950612518</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="13">
         <v>2152.8062418830013</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20">
+        <v>59</v>
+      </c>
+      <c r="B20" s="13">
         <v>741.24668244400027</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="13">
         <v>741.24668244400027</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="13">
         <v>5994.6472325952418</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="13">
         <v>5994.6472325952418</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="13">
         <v>8644.9747456737641</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="13">
         <v>8644.9747456737641</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="13">
         <v>15380.868660713008</v>
       </c>
     </row>
@@ -20942,102 +20772,102 @@
       <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="13">
+        <v>741.24668244400027</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B4">
+      <c r="B5" s="13">
         <v>741.24668244400027</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5">
-        <v>741.24668244400027</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>230</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="13">
         <v>741.24668244400027</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="13">
+        <v>5994.6472325952418</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B7">
+      <c r="B8" s="13">
         <v>5994.6472325952418</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8">
-        <v>5994.6472325952418</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>230</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="13">
         <v>5994.6472325952418</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="13">
+        <v>8644.9747456737641</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B10">
+      <c r="B11" s="13">
         <v>8644.9747456737641</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11">
-        <v>8644.9747456737641</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>110</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="13">
         <v>8644.9747456737641</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13">
+        <v>59</v>
+      </c>
+      <c r="B13" s="13">
         <v>15380.868660713006</v>
       </c>
     </row>
@@ -21050,29 +20880,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77421B50-6F1F-4D62-BA59-D66917AA062E}">
   <dimension ref="B1:K5"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="21" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
@@ -21084,9 +20914,9 @@
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
     </row>
-    <row r="3" spans="2:11" s="2" customFormat="1" ht="28.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" s="2" customFormat="1" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
@@ -21116,7 +20946,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="5"/>
       <c r="E4" t="s">
         <v>8</v>
@@ -21128,7 +20958,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="6"/>
       <c r="E5" t="s">
         <v>9</v>
@@ -21161,54 +20991,54 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
         <v>73</v>
       </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" t="s">
+        <v>75</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>0</v>
       </c>
@@ -21222,7 +21052,7 @@
         <v>7.2340501901582756E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>1</v>
       </c>
@@ -21236,7 +21066,7 @@
         <v>7.9574552091741038E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>2</v>
       </c>
@@ -21250,7 +21080,7 @@
         <v>8.753200730091515E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>3</v>
       </c>
@@ -21264,7 +21094,7 @@
         <v>9.6285208031006677E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>4</v>
       </c>
@@ -21278,7 +21108,7 @@
         <v>1.0591372883410735E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>5</v>
       </c>
@@ -21292,7 +21122,7 @@
         <v>1.165051017175181E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>6</v>
       </c>
@@ -21306,7 +21136,7 @@
         <v>1.2815561188926991E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>7</v>
       </c>
@@ -21320,7 +21150,7 @@
         <v>1.4097117307819692E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>8</v>
       </c>
@@ -21334,7 +21164,7 @@
         <v>1.5506829038601662E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>9</v>
       </c>
@@ -21348,7 +21178,7 @@
         <v>1.7057511942461829E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>10</v>
       </c>
@@ -21362,9 +21192,9 @@
         <v>1.8763263136708014E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16">
         <v>259.82338852073474</v>
@@ -21389,42 +21219,42 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>0</v>
       </c>
@@ -21432,7 +21262,7 @@
         <v>5.0271800432839848</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>1</v>
       </c>
@@ -21440,7 +21270,7 @@
         <v>5.5298980476123836</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>2</v>
       </c>
@@ -21448,7 +21278,7 @@
         <v>6.0828878523736218</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>3</v>
       </c>
@@ -21456,7 +21286,7 @@
         <v>6.6911766376109849</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>4</v>
       </c>
@@ -21464,7 +21294,7 @@
         <v>7.3602943013720843</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>5</v>
       </c>
@@ -21472,7 +21302,7 @@
         <v>8.096323731509294</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>6</v>
       </c>
@@ -21480,7 +21310,7 @@
         <v>8.9059561046602234</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>7</v>
       </c>
@@ -21488,7 +21318,7 @@
         <v>9.7965517151262471</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>8</v>
       </c>
@@ -21496,7 +21326,7 @@
         <v>10.776206886638873</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>9</v>
       </c>
@@ -21504,7 +21334,7 @@
         <v>11.853827575302761</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>10</v>
       </c>
@@ -21512,9 +21342,9 @@
         <v>13.039210332833038</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16">
         <v>93.15951322832349</v>

</xml_diff>